<commit_message>
add spreadsheet operation functions
</commit_message>
<xml_diff>
--- a/test/values.xlsx
+++ b/test/values.xlsx
@@ -1,46 +1,57 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF2D680D-D502-44E0-BCF9-0BA5582EE82A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\imai\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C2CFFC-D566-4EF1-BF48-44BB20C6E6A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>test</t>
   </si>
+  <si>
+    <t>sheet2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>sheet3</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -86,7 +97,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -384,52 +395,90 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <f ca="1">NOW()</f>
-        <v>44300.615062152778</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
+        <v>44305.692058333334</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A4" s="2">
         <v>44300</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A6" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC10C6DC-E371-4A70-9BE9-A80CD759444F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05A965B5-69D9-49BA-8245-EEC26D9BD9EB}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>